<commit_message>
Presentation notebook and docs
</commit_message>
<xml_diff>
--- a/tests/base_assumptions_annuity.xlsx
+++ b/tests/base_assumptions_annuity.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="22515" windowHeight="11070" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="22515" windowHeight="11070"/>
   </bookViews>
   <sheets>
     <sheet name="MORTALITY (0-&gt;3)" sheetId="1" r:id="rId1"/>
@@ -403,8 +403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C124"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -3031,7 +3031,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>

</xml_diff>